<commit_message>
Update Test Report Triple Color
</commit_message>
<xml_diff>
--- a/03. Engineering/036. Testing/Test Report/pLED_TripleColors_TestReport_v1.0.xlsx
+++ b/03. Engineering/036. Testing/Test Report/pLED_TripleColors_TestReport_v1.0.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Before Solder" sheetId="1" r:id="rId1"/>
     <sheet name="After Solder" sheetId="4" r:id="rId2"/>
     <sheet name="After Programing" sheetId="5" r:id="rId3"/>
+    <sheet name="Functional Testing" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="88">
   <si>
     <t xml:space="preserve">TestCase ID </t>
   </si>
@@ -40,12 +41,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>pLED_Dual_001</t>
-  </si>
-  <si>
-    <t>pLED_Dual_002</t>
   </si>
   <si>
     <t>Hall</t>
@@ -63,24 +58,6 @@
 Hall work OK</t>
   </si>
   <si>
-    <t>pLED_Dual_003</t>
-  </si>
-  <si>
-    <t>pLED_Dual_004</t>
-  </si>
-  <si>
-    <t>pLED_Dual_005</t>
-  </si>
-  <si>
-    <t>pLED_Dual_006</t>
-  </si>
-  <si>
-    <t>pLED_Dual_007</t>
-  </si>
-  <si>
-    <t>pLED_Dual_008</t>
-  </si>
-  <si>
     <t>RF Module</t>
   </si>
   <si>
@@ -144,52 +121,158 @@
     <t>Action</t>
   </si>
   <si>
-    <t>pLED_Dual_009</t>
-  </si>
-  <si>
-    <t>pLED_Dual_010</t>
-  </si>
-  <si>
-    <t>pLED_Dual_011</t>
-  </si>
-  <si>
-    <t>pLED_Dual_012</t>
-  </si>
-  <si>
-    <t>pLED_Dual_013</t>
-  </si>
-  <si>
-    <t>pLED_Dual_014</t>
-  </si>
-  <si>
-    <t>pLED_Dual_015</t>
-  </si>
-  <si>
-    <t>pLED_Dual_016</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0017</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0018</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0019</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0020</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0021</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0022</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0023</t>
-  </si>
-  <si>
-    <t>pLED_Dual_0024</t>
+    <t xml:space="preserve">User press button "A" on RF control 
+</t>
+  </si>
+  <si>
+    <t>Display Analog Clock</t>
+  </si>
+  <si>
+    <t>Display Real Time</t>
+  </si>
+  <si>
+    <t>Matching Image Design</t>
+  </si>
+  <si>
+    <t>Clock display smoothly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User press button "B" on RF control 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User press button "C" on RF control 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User press button "D" on RF control 
+</t>
+  </si>
+  <si>
+    <t>Display Digital Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Image </t>
+  </si>
+  <si>
+    <t>Display Text</t>
+  </si>
+  <si>
+    <t>Text display smoothly</t>
+  </si>
+  <si>
+    <t>Image display smoothly</t>
+  </si>
+  <si>
+    <t>pLED_Triple_001</t>
+  </si>
+  <si>
+    <t>pLED_Triple_002</t>
+  </si>
+  <si>
+    <t>pLED_Triple_003</t>
+  </si>
+  <si>
+    <t>pLED_Triple_004</t>
+  </si>
+  <si>
+    <t>pLED_Triple_005</t>
+  </si>
+  <si>
+    <t>pLED_Triple_006</t>
+  </si>
+  <si>
+    <t>pLED_Triple_007</t>
+  </si>
+  <si>
+    <t>pLED_Triple_008</t>
+  </si>
+  <si>
+    <t>pLED_Triple_009</t>
+  </si>
+  <si>
+    <t>pLED_Triple_010</t>
+  </si>
+  <si>
+    <t>pLED_Triple_011</t>
+  </si>
+  <si>
+    <t>pLED_Triple_012</t>
+  </si>
+  <si>
+    <t>pLED_Triple_013</t>
+  </si>
+  <si>
+    <t>pLED_Triple_014</t>
+  </si>
+  <si>
+    <t>pLED_Triple_015</t>
+  </si>
+  <si>
+    <t>pLED_Triple_016</t>
+  </si>
+  <si>
+    <t>pLED_Triple_017</t>
+  </si>
+  <si>
+    <t>pLED_Triple_018</t>
+  </si>
+  <si>
+    <t>pLED_Triple_019</t>
+  </si>
+  <si>
+    <t>pLED_Triple_020</t>
+  </si>
+  <si>
+    <t>pLED_Triple_021</t>
+  </si>
+  <si>
+    <t>pLED_Triple_022</t>
+  </si>
+  <si>
+    <t>pLED_Triple_023</t>
+  </si>
+  <si>
+    <t>pLED_Triple_024</t>
+  </si>
+  <si>
+    <t>pLED_Triple_025</t>
+  </si>
+  <si>
+    <t>pLED_Triple_026</t>
+  </si>
+  <si>
+    <t>pLED_Triple_027</t>
+  </si>
+  <si>
+    <t>pLED_Triple_028</t>
+  </si>
+  <si>
+    <t>pLED_Triple_029</t>
+  </si>
+  <si>
+    <t>pLED_Triple_030</t>
+  </si>
+  <si>
+    <t>pLED_Triple_031</t>
+  </si>
+  <si>
+    <t>pLED_Triple_032</t>
+  </si>
+  <si>
+    <t>pLED_Triple_033</t>
+  </si>
+  <si>
+    <t>pLED_Triple_034</t>
+  </si>
+  <si>
+    <t>pLED_Triple_035</t>
+  </si>
+  <si>
+    <t>pLED_Triple_036</t>
+  </si>
+  <si>
+    <t>pLED_Triple_037</t>
   </si>
   <si>
     <t>OK</t>
@@ -201,22 +284,22 @@
     <t>TungNT</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>10/16 
+Led Connect</t>
+  </si>
+  <si>
     <t>LongNT</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>Cannot 
+Programing</t>
   </si>
   <si>
     <t>Fail after
 solder</t>
-  </si>
-  <si>
-    <t>10/16 
-Led Connect</t>
-  </si>
-  <si>
-    <t>Cannot 
-Programing</t>
   </si>
 </sst>
 </file>
@@ -265,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -301,6 +384,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -323,21 +443,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -345,14 +470,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,7 +780,7 @@
   <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,192 +823,192 @@
     </row>
     <row r="3" spans="2:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="7">
+        <v>81</v>
+      </c>
+      <c r="H3" s="11">
         <v>41659</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="7">
+        <v>81</v>
+      </c>
+      <c r="H4" s="11">
         <v>41659</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="7">
+        <v>81</v>
+      </c>
+      <c r="H5" s="11">
         <v>41659</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="7">
+        <v>81</v>
+      </c>
+      <c r="H6" s="11">
         <v>41659</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="7">
+        <v>81</v>
+      </c>
+      <c r="H7" s="11">
         <v>41659</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="7">
+        <v>81</v>
+      </c>
+      <c r="H8" s="11">
         <v>41659</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="7">
+        <v>81</v>
+      </c>
+      <c r="H9" s="11">
         <v>41659</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="7">
+        <v>81</v>
+      </c>
+      <c r="H10" s="11">
         <v>41659</v>
       </c>
       <c r="I10" s="1"/>
@@ -902,7 +1024,7 @@
   <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="F3" sqref="F3:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +1036,6 @@
     <col min="6" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="13.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -946,194 +1067,194 @@
     </row>
     <row r="3" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>54</v>
+        <v>27</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="7">
+        <v>82</v>
+      </c>
+      <c r="H3" s="11">
         <v>41695</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>54</v>
+        <v>27</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="7">
+        <v>82</v>
+      </c>
+      <c r="H4" s="11">
         <v>41695</v>
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="2:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="13">
+    <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="14">
         <v>41695</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="11">
+        <v>41695</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="16">
+        <v>41695</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="7">
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="16">
         <v>41695</v>
       </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="17">
-        <v>41695</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="17">
-        <v>41695</v>
-      </c>
-      <c r="I8" s="14"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="7">
+        <v>82</v>
+      </c>
+      <c r="H9" s="11">
         <v>41695</v>
       </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="7">
+        <v>82</v>
+      </c>
+      <c r="H10" s="11">
         <v>41695</v>
       </c>
       <c r="I10" s="4"/>
@@ -1148,20 +1269,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="13.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1191,216 +1312,462 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="7">
+        <v>85</v>
+      </c>
+      <c r="H3" s="11">
         <v>41697</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="11">
+        <v>41697</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="11">
         <v>41697</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="7">
-        <v>41697</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="7">
+        <v>85</v>
+      </c>
+      <c r="H6" s="11">
         <v>41698</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="7">
+        <v>85</v>
+      </c>
+      <c r="H7" s="11">
         <v>41699</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="7">
+        <v>85</v>
+      </c>
+      <c r="H8" s="11">
         <v>41700</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="7">
+        <v>85</v>
+      </c>
+      <c r="H9" s="11">
         <v>41701</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="7">
+        <v>85</v>
+      </c>
+      <c r="H10" s="11">
         <v>41703</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>